<commit_message>
Añado Tablas para el informe
</commit_message>
<xml_diff>
--- a/presupuesto/PRESUPUESTO_CURSO_EDIF_PRIM_2018.xlsx
+++ b/presupuesto/PRESUPUESTO_CURSO_EDIF_PRIM_2018.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mleal\Desktop\proyecto-CI6501\presupuesto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Desktop\proyecto edificios\proyecto-CI6501\presupuesto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B5323C-754C-4615-909E-46BDD2ADCD3B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8796426-BD37-4782-B87A-BE8ADECF721F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto Original" sheetId="1" r:id="rId1"/>
     <sheet name="GG" sheetId="2" r:id="rId2"/>
     <sheet name="Personal CD" sheetId="7" r:id="rId3"/>
+    <sheet name="Tablas informe " sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="899">
   <si>
     <t>ITEMIZACION DEL PRESUPUESTO</t>
   </si>
@@ -2658,20 +2659,94 @@
   </si>
   <si>
     <t>IVA 19%</t>
+  </si>
+  <si>
+    <t>Instalación de Faenas</t>
+  </si>
+  <si>
+    <t>Partidas</t>
+  </si>
+  <si>
+    <t>Total CLP</t>
+  </si>
+  <si>
+    <t>Total UF</t>
+  </si>
+  <si>
+    <t>Obra gruesa</t>
+  </si>
+  <si>
+    <t>Terminaciones</t>
+  </si>
+  <si>
+    <t>Partidas Generales</t>
+  </si>
+  <si>
+    <t>Otras Partidas</t>
+  </si>
+  <si>
+    <t>Total Costo Directo</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>\$/MES</t>
+  </si>
+  <si>
+    <t>GASTOS agua mes ( \$ PROMEDIO)</t>
+  </si>
+  <si>
+    <t>Gastos Generales</t>
+  </si>
+  <si>
+    <t>Trabajadores y otros gastos</t>
+  </si>
+  <si>
+    <t>Servicios de Comunicación</t>
+  </si>
+  <si>
+    <t>Caja Chica</t>
+  </si>
+  <si>
+    <t>Total Mensual CLP</t>
+  </si>
+  <si>
+    <t>TOTAL G.G.</t>
+  </si>
+  <si>
+    <t>Imprevisto (8\%)</t>
+  </si>
+  <si>
+    <t>Utilidad (10\%)</t>
+  </si>
+  <si>
+    <t>ADM Central (2\%)</t>
+  </si>
+  <si>
+    <t>Costo total Obra</t>
+  </si>
+  <si>
+    <t>Csoto Directo</t>
+  </si>
+  <si>
+    <t>IVA (19\%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="170" formatCode="0.000%"/>
+  <numFmts count="7">
+    <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
+    <numFmt numFmtId="168" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2869,6 +2944,27 @@
       <name val="Times New Roman"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -2938,7 +3034,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="59">
+  <borders count="84">
     <border>
       <left/>
       <right/>
@@ -3690,13 +3786,337 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="249">
+  <cellXfs count="338">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3791,7 +4211,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3812,7 +4232,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3830,7 +4250,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3848,7 +4268,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3872,7 +4292,7 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3887,7 +4307,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3908,7 +4328,7 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3923,7 +4343,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3932,7 +4352,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3944,13 +4364,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3971,7 +4391,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3983,10 +4403,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4010,7 +4430,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4022,16 +4442,16 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4116,13 +4536,13 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4180,9 +4600,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4192,9 +4609,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4204,9 +4618,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4216,9 +4627,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4228,9 +4636,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4240,17 +4645,8 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4273,9 +4669,6 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
@@ -4336,29 +4729,44 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="11"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="11"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="11"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -4372,41 +4780,271 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="41" fontId="24" fillId="0" borderId="61" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="24" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="26" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="26" fillId="0" borderId="69" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="24" fillId="0" borderId="66" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="24" fillId="0" borderId="67" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="24" fillId="0" borderId="68" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="26" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="26" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="60" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="24" fillId="0" borderId="60" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="24" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="24" fillId="0" borderId="62" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="63" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="64" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="24" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="24" fillId="0" borderId="57" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="26" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="26" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="26" fillId="0" borderId="57" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="24" fillId="0" borderId="61" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="24" fillId="0" borderId="65" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="24" fillId="0" borderId="69" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+  <cellStyles count="4">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+    <cellStyle name="Moneda [0]" xfId="3" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4492,7 +5130,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4559,7 +5197,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4753,7 +5391,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4790,7 +5428,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="746759488"/>
@@ -4869,7 +5507,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4907,7 +5545,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="279484656"/>
@@ -4955,7 +5593,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5613,7 +6251,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5917,7 +6555,7 @@
       <selection pane="bottomLeft" activeCell="E488" sqref="E488"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" style="2" customWidth="1"/>
@@ -5934,15 +6572,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="230" t="s">
+      <c r="A1" s="222" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="230"/>
-      <c r="C1" s="230"/>
-      <c r="D1" s="230"/>
-      <c r="E1" s="230"/>
-      <c r="F1" s="230"/>
-      <c r="G1" s="230"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -5974,10 +6612,10 @@
       <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="231" t="s">
+      <c r="D4" s="223" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="232" t="s">
+      <c r="E4" s="224" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="20" t="s">
@@ -5991,8 +6629,8 @@
       <c r="A5" s="17"/>
       <c r="B5" s="21"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="231"/>
-      <c r="E5" s="232"/>
+      <c r="D5" s="223"/>
+      <c r="E5" s="224"/>
       <c r="F5" s="23" t="s">
         <v>9</v>
       </c>
@@ -6356,10 +6994,10 @@
     </row>
     <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
-      <c r="B28" s="227" t="s">
+      <c r="B28" s="225" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="227"/>
+      <c r="C28" s="225"/>
       <c r="D28" s="26"/>
       <c r="E28" s="27"/>
       <c r="F28" s="26"/>
@@ -7892,10 +8530,10 @@
       <c r="I130" s="83"/>
     </row>
     <row r="131" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="228" t="s">
+      <c r="B131" s="226" t="s">
         <v>170</v>
       </c>
-      <c r="C131" s="228"/>
+      <c r="C131" s="226"/>
       <c r="D131" s="82" t="s">
         <v>109</v>
       </c>
@@ -7906,10 +8544,10 @@
       <c r="G131" s="69"/>
     </row>
     <row r="132" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="228" t="s">
+      <c r="B132" s="226" t="s">
         <v>171</v>
       </c>
-      <c r="C132" s="228"/>
+      <c r="C132" s="226"/>
       <c r="D132" s="82" t="s">
         <v>109</v>
       </c>
@@ -8215,7 +8853,7 @@
       </c>
       <c r="F154" s="67"/>
       <c r="G154" s="69"/>
-      <c r="I154" s="229" t="s">
+      <c r="I154" s="227" t="s">
         <v>190</v>
       </c>
     </row>
@@ -8232,7 +8870,7 @@
       </c>
       <c r="F155" s="67"/>
       <c r="G155" s="69"/>
-      <c r="I155" s="229"/>
+      <c r="I155" s="227"/>
     </row>
     <row r="156" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="78"/>
@@ -8247,7 +8885,7 @@
       </c>
       <c r="F156" s="67"/>
       <c r="G156" s="69"/>
-      <c r="I156" s="229"/>
+      <c r="I156" s="227"/>
     </row>
     <row r="157" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="78"/>
@@ -8262,7 +8900,7 @@
       </c>
       <c r="F157" s="67"/>
       <c r="G157" s="69"/>
-      <c r="I157" s="229"/>
+      <c r="I157" s="227"/>
     </row>
     <row r="158" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="78"/>
@@ -8277,7 +8915,7 @@
       </c>
       <c r="F158" s="67"/>
       <c r="G158" s="69"/>
-      <c r="I158" s="229"/>
+      <c r="I158" s="227"/>
     </row>
     <row r="159" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="29" t="s">
@@ -10445,7 +11083,7 @@
       </c>
       <c r="F323" s="61"/>
       <c r="G323" s="61"/>
-      <c r="I323" s="229" t="s">
+      <c r="I323" s="227" t="s">
         <v>324</v>
       </c>
     </row>
@@ -10464,7 +11102,7 @@
       </c>
       <c r="F324" s="61"/>
       <c r="G324" s="61"/>
-      <c r="I324" s="229"/>
+      <c r="I324" s="227"/>
     </row>
     <row r="325" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B325" s="58" t="s">
@@ -10481,7 +11119,7 @@
       </c>
       <c r="F325" s="61"/>
       <c r="G325" s="61"/>
-      <c r="I325" s="229"/>
+      <c r="I325" s="227"/>
     </row>
     <row r="326" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B326" s="58" t="s">
@@ -10498,7 +11136,7 @@
       </c>
       <c r="F326" s="61"/>
       <c r="G326" s="61"/>
-      <c r="I326" s="229"/>
+      <c r="I326" s="227"/>
     </row>
     <row r="327" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B327" s="94" t="s">
@@ -11134,7 +11772,7 @@
       <c r="E370" s="27"/>
       <c r="F370" s="26"/>
       <c r="G370" s="28"/>
-      <c r="I370" s="229" t="s">
+      <c r="I370" s="227" t="s">
         <v>396</v>
       </c>
     </row>
@@ -11151,7 +11789,7 @@
       <c r="E371" s="96"/>
       <c r="F371" s="55"/>
       <c r="G371" s="57"/>
-      <c r="I371" s="229"/>
+      <c r="I371" s="227"/>
     </row>
     <row r="372" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B372" s="58" t="s">
@@ -11169,7 +11807,7 @@
       </c>
       <c r="F372" s="61"/>
       <c r="G372" s="61"/>
-      <c r="I372" s="229"/>
+      <c r="I372" s="227"/>
     </row>
     <row r="373" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B373" s="78"/>
@@ -11184,7 +11822,7 @@
       </c>
       <c r="F373" s="67"/>
       <c r="G373" s="69"/>
-      <c r="I373" s="229"/>
+      <c r="I373" s="227"/>
     </row>
     <row r="374" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B374" s="78"/>
@@ -11199,7 +11837,7 @@
       </c>
       <c r="F374" s="67"/>
       <c r="G374" s="69"/>
-      <c r="I374" s="229"/>
+      <c r="I374" s="227"/>
     </row>
     <row r="375" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B375" s="78"/>
@@ -11214,7 +11852,7 @@
       </c>
       <c r="F375" s="67"/>
       <c r="G375" s="69"/>
-      <c r="I375" s="229"/>
+      <c r="I375" s="227"/>
     </row>
     <row r="376" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B376" s="78"/>
@@ -11229,7 +11867,7 @@
       </c>
       <c r="F376" s="67"/>
       <c r="G376" s="69"/>
-      <c r="I376" s="229"/>
+      <c r="I376" s="227"/>
     </row>
     <row r="377" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B377" s="78"/>
@@ -12795,7 +13433,7 @@
       <c r="E488" s="35"/>
       <c r="F488" s="33"/>
       <c r="G488" s="34"/>
-      <c r="I488" s="229" t="s">
+      <c r="I488" s="227" t="s">
         <v>553</v>
       </c>
     </row>
@@ -12817,7 +13455,7 @@
         <v>556</v>
       </c>
       <c r="H489" s="83"/>
-      <c r="I489" s="229"/>
+      <c r="I489" s="227"/>
     </row>
     <row r="490" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B490" s="78"/>
@@ -15716,10 +16354,10 @@
       <c r="G704" s="34"/>
     </row>
     <row r="705" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B705" s="227" t="s">
+      <c r="B705" s="225" t="s">
         <v>770</v>
       </c>
-      <c r="C705" s="227"/>
+      <c r="C705" s="225"/>
       <c r="D705" s="26"/>
       <c r="E705" s="27"/>
       <c r="F705" s="26"/>
@@ -15810,28 +16448,28 @@
       <c r="G711" s="61"/>
     </row>
     <row r="712" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B712" s="227" t="s">
+      <c r="B712" s="225" t="s">
         <v>780</v>
       </c>
-      <c r="C712" s="227"/>
+      <c r="C712" s="225"/>
       <c r="D712" s="26"/>
       <c r="E712" s="27"/>
       <c r="F712" s="26"/>
       <c r="G712" s="28"/>
     </row>
     <row r="713" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B713" s="225"/>
-      <c r="C713" s="225"/>
+      <c r="B713" s="228"/>
+      <c r="C713" s="228"/>
       <c r="D713" s="52"/>
       <c r="E713" s="103"/>
       <c r="F713" s="52"/>
       <c r="G713" s="53"/>
     </row>
     <row r="714" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B714" s="227" t="s">
+      <c r="B714" s="225" t="s">
         <v>781</v>
       </c>
-      <c r="C714" s="227"/>
+      <c r="C714" s="225"/>
       <c r="D714" s="26"/>
       <c r="E714" s="27"/>
       <c r="F714" s="26"/>
@@ -15998,45 +16636,35 @@
       <c r="G724" s="61"/>
     </row>
     <row r="725" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B725" s="227" t="s">
+      <c r="B725" s="225" t="s">
         <v>802</v>
       </c>
-      <c r="C725" s="227"/>
+      <c r="C725" s="225"/>
       <c r="D725" s="26"/>
       <c r="E725" s="27"/>
       <c r="F725" s="26"/>
       <c r="G725" s="28"/>
     </row>
     <row r="726" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B726" s="225"/>
-      <c r="C726" s="225"/>
-      <c r="D726" s="225"/>
-      <c r="E726" s="225"/>
-      <c r="F726" s="225"/>
-      <c r="G726" s="225"/>
+      <c r="B726" s="228"/>
+      <c r="C726" s="228"/>
+      <c r="D726" s="228"/>
+      <c r="E726" s="228"/>
+      <c r="F726" s="228"/>
+      <c r="G726" s="228"/>
     </row>
     <row r="727" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B727" s="226" t="s">
+      <c r="B727" s="229" t="s">
         <v>803</v>
       </c>
-      <c r="C727" s="226"/>
-      <c r="D727" s="226"/>
-      <c r="E727" s="226"/>
-      <c r="F727" s="226"/>
-      <c r="G727" s="226"/>
+      <c r="C727" s="229"/>
+      <c r="D727" s="229"/>
+      <c r="E727" s="229"/>
+      <c r="F727" s="229"/>
+      <c r="G727" s="229"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="I154:I158"/>
-    <mergeCell ref="I323:I326"/>
-    <mergeCell ref="I370:I376"/>
-    <mergeCell ref="I488:I489"/>
     <mergeCell ref="B726:G726"/>
     <mergeCell ref="B727:G727"/>
     <mergeCell ref="B705:C705"/>
@@ -16044,6 +16672,16 @@
     <mergeCell ref="B713:C713"/>
     <mergeCell ref="B714:C714"/>
     <mergeCell ref="B725:C725"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="I154:I158"/>
+    <mergeCell ref="I323:I326"/>
+    <mergeCell ref="I370:I376"/>
+    <mergeCell ref="I488:I489"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B131:C131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -16054,11 +16692,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T54" sqref="T54:U54"/>
+    <sheetView topLeftCell="K31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X46" sqref="X46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="128" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" style="145" customWidth="1"/>
@@ -16078,7 +16716,7 @@
     <col min="1025" max="16384" width="9.33203125" style="122"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="120"/>
       <c r="B1" s="129"/>
       <c r="C1" s="129"/>
@@ -16086,7 +16724,7 @@
       <c r="E1" s="129"/>
       <c r="F1" s="121"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="123"/>
       <c r="B2" s="130" t="s">
         <v>804</v>
@@ -16096,15 +16734,35 @@
       <c r="E2" s="129"/>
       <c r="F2" s="121"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="124"/>
       <c r="B3" s="130"/>
       <c r="C3" s="131"/>
       <c r="D3" s="131"/>
       <c r="E3" s="131"/>
       <c r="F3" s="121"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R3" s="122">
+        <f>SUM(I22:I35)</f>
+        <v>15</v>
+      </c>
+      <c r="S3" s="122">
+        <f t="shared" ref="S3:V3" si="0">SUM(J22:J35)</f>
+        <v>20</v>
+      </c>
+      <c r="T3" s="122">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="U3" s="122">
+        <f t="shared" si="0"/>
+        <v>21.25</v>
+      </c>
+      <c r="V3" s="122">
+        <f t="shared" si="0"/>
+        <v>24.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="125"/>
       <c r="B4" s="132" t="s">
         <v>805</v>
@@ -16118,7 +16776,7 @@
       <c r="E4" s="133"/>
       <c r="F4" s="126"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="127"/>
       <c r="B5" s="134"/>
       <c r="C5" s="133" t="s">
@@ -16132,7 +16790,7 @@
       </c>
       <c r="F5" s="126"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="127"/>
       <c r="B6" s="133"/>
       <c r="C6" s="133"/>
@@ -16140,7 +16798,7 @@
       <c r="E6" s="133"/>
       <c r="F6" s="126"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="123"/>
       <c r="B7" s="155" t="s">
         <v>810</v>
@@ -16158,7 +16816,7 @@
       <c r="G7" s="154"/>
       <c r="H7" s="158"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="127"/>
       <c r="B8" s="155" t="s">
         <v>811</v>
@@ -16174,7 +16832,7 @@
       </c>
       <c r="F8" s="126"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="127"/>
       <c r="B9" s="155" t="s">
         <v>812</v>
@@ -16190,7 +16848,7 @@
       </c>
       <c r="F9" s="126"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="125"/>
       <c r="B10" s="155" t="s">
         <v>813</v>
@@ -16206,7 +16864,7 @@
       </c>
       <c r="F10" s="126"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="127"/>
       <c r="B11" s="133" t="s">
         <v>814</v>
@@ -16222,7 +16880,7 @@
       </c>
       <c r="F11" s="126"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="127"/>
       <c r="B12" s="133" t="s">
         <v>815</v>
@@ -16238,7 +16896,7 @@
       </c>
       <c r="F12" s="126"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="125"/>
       <c r="B13" s="133" t="s">
         <v>816</v>
@@ -16254,7 +16912,7 @@
       </c>
       <c r="F13" s="126"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="127"/>
       <c r="B14" s="133" t="s">
         <v>817</v>
@@ -16270,7 +16928,7 @@
       </c>
       <c r="F14" s="126"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="127"/>
       <c r="B15" s="133" t="s">
         <v>818</v>
@@ -16286,7 +16944,7 @@
       </c>
       <c r="F15" s="126"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="125"/>
       <c r="B16" s="133" t="s">
         <v>819</v>
@@ -16351,34 +17009,34 @@
         <v>111</v>
       </c>
       <c r="F19" s="126"/>
-      <c r="T19" s="171" t="s">
+      <c r="T19" s="291" t="s">
         <v>809</v>
       </c>
-      <c r="U19" s="167" t="s">
+      <c r="U19" s="292" t="s">
         <v>833</v>
       </c>
-      <c r="V19" s="163" t="s">
+      <c r="V19" s="293" t="s">
         <v>834</v>
       </c>
-      <c r="W19" s="163" t="s">
+      <c r="W19" s="293" t="s">
         <v>835</v>
       </c>
-      <c r="X19" s="163" t="s">
+      <c r="X19" s="293" t="s">
         <v>836</v>
       </c>
-      <c r="Y19" s="163" t="s">
+      <c r="Y19" s="293" t="s">
         <v>837</v>
       </c>
-      <c r="Z19" s="163" t="s">
+      <c r="Z19" s="293" t="s">
         <v>838</v>
       </c>
-      <c r="AA19" s="163" t="s">
+      <c r="AA19" s="293" t="s">
         <v>839</v>
       </c>
-      <c r="AB19" s="175" t="s">
+      <c r="AB19" s="294" t="s">
         <v>840</v>
       </c>
-      <c r="AC19" s="179" t="s">
+      <c r="AC19" s="295" t="s">
         <v>857</v>
       </c>
     </row>
@@ -16398,44 +17056,44 @@
       </c>
       <c r="F20" s="126"/>
       <c r="G20" s="156"/>
-      <c r="H20" s="193" t="s">
+      <c r="H20" s="185" t="s">
         <v>809</v>
       </c>
-      <c r="I20" s="186" t="s">
+      <c r="I20" s="297" t="s">
         <v>833</v>
       </c>
-      <c r="J20" s="187" t="s">
+      <c r="J20" s="298" t="s">
         <v>834</v>
       </c>
-      <c r="K20" s="187" t="s">
+      <c r="K20" s="298" t="s">
         <v>835</v>
       </c>
-      <c r="L20" s="187" t="s">
+      <c r="L20" s="298" t="s">
         <v>836</v>
       </c>
-      <c r="M20" s="187" t="s">
+      <c r="M20" s="298" t="s">
         <v>837</v>
       </c>
-      <c r="N20" s="187" t="s">
+      <c r="N20" s="298" t="s">
         <v>838</v>
       </c>
-      <c r="O20" s="187" t="s">
+      <c r="O20" s="298" t="s">
         <v>839</v>
       </c>
-      <c r="P20" s="198" t="s">
+      <c r="P20" s="299" t="s">
         <v>840</v>
       </c>
-      <c r="Q20" s="203" t="s">
+      <c r="Q20" s="194" t="s">
         <v>857</v>
       </c>
-      <c r="S20" s="164" t="s">
+      <c r="S20" s="163" t="s">
         <v>849</v>
       </c>
-      <c r="T20" s="172">
+      <c r="T20" s="169">
         <f>$E$8</f>
         <v>259</v>
       </c>
-      <c r="U20" s="168">
+      <c r="U20" s="166">
         <v>1</v>
       </c>
       <c r="V20" s="160">
@@ -16446,42 +17104,42 @@
       <c r="Y20" s="160"/>
       <c r="Z20" s="160"/>
       <c r="AA20" s="160"/>
-      <c r="AB20" s="176"/>
-      <c r="AC20" s="180">
-        <f t="shared" ref="AC20:AC27" si="0">SUM(U20:AB20)*T20</f>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="175">
+        <f t="shared" ref="AC20:AC27" si="1">SUM(U20:AB20)*T20</f>
         <v>518</v>
       </c>
     </row>
     <row r="21" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="127"/>
-      <c r="B21" s="233" t="s">
+      <c r="B21" s="231" t="s">
         <v>824</v>
       </c>
-      <c r="C21" s="234"/>
-      <c r="D21" s="234"/>
-      <c r="E21" s="235"/>
+      <c r="C21" s="232"/>
+      <c r="D21" s="232"/>
+      <c r="E21" s="233"/>
       <c r="F21" s="126"/>
-      <c r="G21" s="190" t="s">
+      <c r="G21" s="182" t="s">
         <v>832</v>
       </c>
-      <c r="H21" s="194"/>
-      <c r="I21" s="195"/>
-      <c r="J21" s="195"/>
-      <c r="K21" s="195"/>
-      <c r="L21" s="195"/>
-      <c r="M21" s="195"/>
-      <c r="N21" s="195"/>
-      <c r="O21" s="195"/>
-      <c r="P21" s="195"/>
-      <c r="Q21" s="204"/>
-      <c r="S21" s="165" t="s">
+      <c r="H21" s="186"/>
+      <c r="I21" s="187"/>
+      <c r="J21" s="187"/>
+      <c r="K21" s="187"/>
+      <c r="L21" s="187"/>
+      <c r="M21" s="187"/>
+      <c r="N21" s="187"/>
+      <c r="O21" s="187"/>
+      <c r="P21" s="187"/>
+      <c r="Q21" s="195"/>
+      <c r="S21" s="164" t="s">
         <v>856</v>
       </c>
-      <c r="T21" s="173">
+      <c r="T21" s="170">
         <f>$E$8</f>
         <v>259</v>
       </c>
-      <c r="U21" s="169"/>
+      <c r="U21" s="167"/>
       <c r="V21" s="161"/>
       <c r="W21" s="161">
         <v>1</v>
@@ -16490,9 +17148,9 @@
       <c r="Y21" s="161"/>
       <c r="Z21" s="161"/>
       <c r="AA21" s="161"/>
-      <c r="AB21" s="177"/>
-      <c r="AC21" s="181">
-        <f t="shared" si="0"/>
+      <c r="AB21" s="173"/>
+      <c r="AC21" s="176">
+        <f t="shared" si="1"/>
         <v>259</v>
       </c>
     </row>
@@ -16510,50 +17168,50 @@
         <v>75</v>
       </c>
       <c r="F22" s="126"/>
-      <c r="G22" s="191" t="str">
+      <c r="G22" s="183" t="str">
         <f>B7</f>
         <v>ADMINSITRADOR CONTRATO</v>
       </c>
-      <c r="H22" s="213">
-        <f t="shared" ref="H22:H27" si="1">E7</f>
+      <c r="H22" s="204">
+        <f>E7</f>
         <v>370</v>
       </c>
-      <c r="I22" s="188">
+      <c r="I22" s="180">
         <v>1</v>
       </c>
-      <c r="J22" s="184">
+      <c r="J22" s="178">
         <v>1</v>
       </c>
-      <c r="K22" s="184">
+      <c r="K22" s="178">
         <v>1</v>
       </c>
-      <c r="L22" s="184">
+      <c r="L22" s="178">
         <v>1</v>
       </c>
-      <c r="M22" s="184">
+      <c r="M22" s="178">
         <v>1</v>
       </c>
-      <c r="N22" s="184">
+      <c r="N22" s="178">
         <v>1</v>
       </c>
-      <c r="O22" s="196">
+      <c r="O22" s="188">
         <v>1</v>
       </c>
-      <c r="P22" s="196">
+      <c r="P22" s="188">
         <v>1</v>
       </c>
-      <c r="Q22" s="209">
+      <c r="Q22" s="200">
         <f t="shared" ref="Q22:Q35" si="2">SUM(I22:P22)*H22</f>
         <v>2960</v>
       </c>
-      <c r="S22" s="165" t="s">
+      <c r="S22" s="164" t="s">
         <v>850</v>
       </c>
-      <c r="T22" s="173">
+      <c r="T22" s="170">
         <f t="shared" ref="T22:T27" si="3">$E$8</f>
         <v>259</v>
       </c>
-      <c r="U22" s="169"/>
+      <c r="U22" s="167"/>
       <c r="V22" s="161"/>
       <c r="W22" s="161"/>
       <c r="X22" s="161">
@@ -16566,9 +17224,9 @@
         <v>0.5</v>
       </c>
       <c r="AA22" s="161"/>
-      <c r="AB22" s="177"/>
-      <c r="AC22" s="181">
-        <f t="shared" si="0"/>
+      <c r="AB22" s="173"/>
+      <c r="AC22" s="176">
+        <f t="shared" si="1"/>
         <v>647.5</v>
       </c>
     </row>
@@ -16586,58 +17244,58 @@
         <v>297</v>
       </c>
       <c r="F23" s="126"/>
-      <c r="G23" s="191" t="str">
+      <c r="G23" s="183" t="str">
         <f>B8</f>
         <v>SUPERVISORES DE TERRENO</v>
       </c>
-      <c r="H23" s="213">
-        <f t="shared" si="1"/>
+      <c r="H23" s="204">
+        <f t="shared" ref="H22:H27" si="5">E8</f>
         <v>259</v>
       </c>
-      <c r="I23" s="188">
-        <f t="shared" ref="I23:P23" si="5">SUM(U20:U27)</f>
+      <c r="I23" s="180">
+        <f t="shared" ref="I23:P23" si="6">SUM(U20:U27)</f>
         <v>1</v>
       </c>
-      <c r="J23" s="184">
-        <f t="shared" si="5"/>
+      <c r="J23" s="178">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="K23" s="184">
-        <f t="shared" si="5"/>
+      <c r="K23" s="178">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="L23" s="184">
-        <f t="shared" si="5"/>
+      <c r="L23" s="178">
+        <f t="shared" si="6"/>
         <v>1.25</v>
       </c>
-      <c r="M23" s="184">
-        <f t="shared" si="5"/>
+      <c r="M23" s="178">
+        <f t="shared" si="6"/>
         <v>3.25</v>
       </c>
-      <c r="N23" s="184">
-        <f t="shared" si="5"/>
+      <c r="N23" s="178">
+        <f>SUM(Z20:Z27)</f>
         <v>5.25</v>
       </c>
-      <c r="O23" s="196">
-        <f t="shared" si="5"/>
+      <c r="O23" s="188">
+        <f t="shared" si="6"/>
         <v>3.75</v>
       </c>
-      <c r="P23" s="196">
-        <f t="shared" si="5"/>
+      <c r="P23" s="188">
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
-      <c r="Q23" s="209">
+      <c r="Q23" s="200">
         <f t="shared" si="2"/>
         <v>4662</v>
       </c>
-      <c r="S23" s="165" t="s">
+      <c r="S23" s="164" t="s">
         <v>851</v>
       </c>
-      <c r="T23" s="173">
+      <c r="T23" s="170">
         <f t="shared" si="3"/>
         <v>259</v>
       </c>
-      <c r="U23" s="169"/>
+      <c r="U23" s="167"/>
       <c r="V23" s="161"/>
       <c r="W23" s="161"/>
       <c r="X23" s="161">
@@ -16652,9 +17310,9 @@
       <c r="AA23" s="161">
         <v>0.25</v>
       </c>
-      <c r="AB23" s="177"/>
-      <c r="AC23" s="181">
-        <f t="shared" si="0"/>
+      <c r="AB23" s="173"/>
+      <c r="AC23" s="176">
+        <f t="shared" si="1"/>
         <v>647.5</v>
       </c>
     </row>
@@ -16672,35 +17330,35 @@
         <v>6</v>
       </c>
       <c r="F24" s="126"/>
-      <c r="G24" s="191" t="s">
+      <c r="G24" s="183" t="s">
         <v>812</v>
       </c>
-      <c r="H24" s="213">
-        <f t="shared" si="1"/>
+      <c r="H24" s="204">
+        <f t="shared" si="5"/>
         <v>185</v>
       </c>
-      <c r="I24" s="188"/>
-      <c r="J24" s="184">
+      <c r="I24" s="180"/>
+      <c r="J24" s="178">
         <v>1</v>
       </c>
-      <c r="K24" s="184"/>
-      <c r="L24" s="184"/>
-      <c r="M24" s="184"/>
-      <c r="N24" s="184"/>
-      <c r="O24" s="196"/>
-      <c r="P24" s="196"/>
-      <c r="Q24" s="209">
+      <c r="K24" s="178"/>
+      <c r="L24" s="178"/>
+      <c r="M24" s="178"/>
+      <c r="N24" s="178"/>
+      <c r="O24" s="188"/>
+      <c r="P24" s="188"/>
+      <c r="Q24" s="200">
         <f t="shared" si="2"/>
         <v>185</v>
       </c>
-      <c r="S24" s="165" t="s">
+      <c r="S24" s="164" t="s">
         <v>852</v>
       </c>
-      <c r="T24" s="173">
+      <c r="T24" s="170">
         <f t="shared" si="3"/>
         <v>259</v>
       </c>
-      <c r="U24" s="169"/>
+      <c r="U24" s="167"/>
       <c r="V24" s="161"/>
       <c r="W24" s="161"/>
       <c r="X24" s="161"/>
@@ -16713,9 +17371,9 @@
       <c r="AA24" s="161">
         <v>0.5</v>
       </c>
-      <c r="AB24" s="177"/>
-      <c r="AC24" s="181">
-        <f t="shared" si="0"/>
+      <c r="AB24" s="173"/>
+      <c r="AC24" s="176">
+        <f t="shared" si="1"/>
         <v>518</v>
       </c>
     </row>
@@ -16733,50 +17391,50 @@
         <v>8</v>
       </c>
       <c r="F25" s="126"/>
-      <c r="G25" s="191" t="str">
-        <f t="shared" ref="G25:G38" si="6">B10</f>
+      <c r="G25" s="183" t="str">
+        <f t="shared" ref="G25:G38" si="7">B10</f>
         <v>RESPONSABLE MEDIO AMBIENTE</v>
       </c>
-      <c r="H25" s="214">
-        <f t="shared" si="1"/>
+      <c r="H25" s="205">
+        <f t="shared" si="5"/>
         <v>185</v>
       </c>
-      <c r="I25" s="188">
+      <c r="I25" s="180">
         <v>1</v>
       </c>
-      <c r="J25" s="184">
+      <c r="J25" s="178">
         <v>1</v>
       </c>
-      <c r="K25" s="184">
+      <c r="K25" s="178">
         <v>1</v>
       </c>
-      <c r="L25" s="184">
+      <c r="L25" s="178">
         <v>1</v>
       </c>
-      <c r="M25" s="184">
+      <c r="M25" s="178">
         <v>1</v>
       </c>
-      <c r="N25" s="184">
+      <c r="N25" s="178">
         <v>1</v>
       </c>
-      <c r="O25" s="196">
+      <c r="O25" s="188">
         <v>1</v>
       </c>
-      <c r="P25" s="196">
+      <c r="P25" s="188">
         <v>1</v>
       </c>
-      <c r="Q25" s="209">
+      <c r="Q25" s="200">
         <f t="shared" si="2"/>
         <v>1480</v>
       </c>
-      <c r="S25" s="165" t="s">
+      <c r="S25" s="164" t="s">
         <v>853</v>
       </c>
-      <c r="T25" s="173">
+      <c r="T25" s="170">
         <f t="shared" si="3"/>
         <v>259</v>
       </c>
-      <c r="U25" s="169"/>
+      <c r="U25" s="167"/>
       <c r="V25" s="161"/>
       <c r="W25" s="161"/>
       <c r="X25" s="161"/>
@@ -16787,67 +17445,67 @@
       <c r="AA25" s="161">
         <v>1</v>
       </c>
-      <c r="AB25" s="177">
+      <c r="AB25" s="173">
         <v>0.25</v>
       </c>
-      <c r="AC25" s="181">
-        <f t="shared" si="0"/>
+      <c r="AC25" s="176">
+        <f t="shared" si="1"/>
         <v>518</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="125"/>
       <c r="B26" s="137" t="s">
         <v>829</v>
       </c>
       <c r="C26" s="137"/>
       <c r="D26" s="137"/>
-      <c r="E26" s="218"/>
-      <c r="F26" s="219"/>
-      <c r="G26" s="191" t="str">
-        <f t="shared" si="6"/>
+      <c r="E26" s="209"/>
+      <c r="F26" s="210"/>
+      <c r="G26" s="183" t="str">
+        <f t="shared" si="7"/>
         <v>RESPONSABLE SEGURIDAD</v>
       </c>
-      <c r="H26" s="214">
-        <f t="shared" si="1"/>
+      <c r="H26" s="205">
+        <f t="shared" si="5"/>
         <v>185</v>
       </c>
-      <c r="I26" s="188">
+      <c r="I26" s="180">
         <v>1</v>
       </c>
-      <c r="J26" s="184">
+      <c r="J26" s="178">
         <v>1</v>
       </c>
-      <c r="K26" s="184">
+      <c r="K26" s="178">
         <v>1</v>
       </c>
-      <c r="L26" s="184">
+      <c r="L26" s="178">
         <v>1</v>
       </c>
-      <c r="M26" s="184">
+      <c r="M26" s="178">
         <v>1</v>
       </c>
-      <c r="N26" s="184">
+      <c r="N26" s="178">
         <v>1</v>
       </c>
-      <c r="O26" s="196">
+      <c r="O26" s="188">
         <v>1</v>
       </c>
-      <c r="P26" s="196">
+      <c r="P26" s="188">
         <v>1</v>
       </c>
-      <c r="Q26" s="209">
+      <c r="Q26" s="200">
         <f t="shared" si="2"/>
         <v>1480</v>
       </c>
-      <c r="S26" s="165" t="s">
+      <c r="S26" s="164" t="s">
         <v>854</v>
       </c>
-      <c r="T26" s="173">
+      <c r="T26" s="170">
         <f t="shared" si="3"/>
         <v>259</v>
       </c>
-      <c r="U26" s="169"/>
+      <c r="U26" s="167"/>
       <c r="V26" s="161"/>
       <c r="W26" s="161"/>
       <c r="X26" s="161"/>
@@ -16860,67 +17518,67 @@
       <c r="AA26" s="161">
         <v>1</v>
       </c>
-      <c r="AB26" s="177">
+      <c r="AB26" s="173">
         <v>0.5</v>
       </c>
-      <c r="AC26" s="181">
-        <f t="shared" si="0"/>
+      <c r="AC26" s="176">
+        <f t="shared" si="1"/>
         <v>777</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:29" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="127"/>
       <c r="B27" s="138" t="s">
         <v>830</v>
       </c>
       <c r="C27" s="138"/>
       <c r="D27" s="138"/>
-      <c r="E27" s="218"/>
-      <c r="F27" s="219"/>
-      <c r="G27" s="191" t="str">
-        <f t="shared" si="6"/>
+      <c r="E27" s="209"/>
+      <c r="F27" s="210"/>
+      <c r="G27" s="183" t="str">
+        <f t="shared" si="7"/>
         <v>RESPONSABLE GESTION DE CALIDAD</v>
       </c>
-      <c r="H27" s="214">
-        <f t="shared" si="1"/>
+      <c r="H27" s="205">
+        <f t="shared" si="5"/>
         <v>259</v>
       </c>
-      <c r="I27" s="188">
+      <c r="I27" s="180">
         <v>1</v>
       </c>
-      <c r="J27" s="184">
+      <c r="J27" s="178">
         <v>1</v>
       </c>
-      <c r="K27" s="184">
+      <c r="K27" s="178">
         <v>1</v>
       </c>
-      <c r="L27" s="184">
+      <c r="L27" s="178">
         <v>1</v>
       </c>
-      <c r="M27" s="184">
+      <c r="M27" s="178">
         <v>1</v>
       </c>
-      <c r="N27" s="184">
+      <c r="N27" s="178">
         <v>1</v>
       </c>
-      <c r="O27" s="196">
+      <c r="O27" s="188">
         <v>1</v>
       </c>
-      <c r="P27" s="196">
+      <c r="P27" s="188">
         <v>1</v>
       </c>
-      <c r="Q27" s="209">
+      <c r="Q27" s="200">
         <f t="shared" si="2"/>
         <v>2072</v>
       </c>
-      <c r="S27" s="166" t="s">
+      <c r="S27" s="165" t="s">
         <v>855</v>
       </c>
-      <c r="T27" s="174">
+      <c r="T27" s="171">
         <f t="shared" si="3"/>
         <v>259</v>
       </c>
-      <c r="U27" s="170"/>
+      <c r="U27" s="168"/>
       <c r="V27" s="162"/>
       <c r="W27" s="162"/>
       <c r="X27" s="162"/>
@@ -16933,11 +17591,11 @@
       <c r="AA27" s="162">
         <v>1</v>
       </c>
-      <c r="AB27" s="178">
+      <c r="AB27" s="174">
         <v>0.75</v>
       </c>
-      <c r="AC27" s="182">
-        <f t="shared" si="0"/>
+      <c r="AC27" s="177">
+        <f t="shared" si="1"/>
         <v>777</v>
       </c>
     </row>
@@ -16946,41 +17604,41 @@
       <c r="B28" s="139"/>
       <c r="C28" s="129"/>
       <c r="D28" s="129"/>
-      <c r="E28" s="218"/>
-      <c r="F28" s="219"/>
-      <c r="G28" s="191" t="str">
-        <f t="shared" si="6"/>
+      <c r="E28" s="209"/>
+      <c r="F28" s="210"/>
+      <c r="G28" s="183" t="str">
+        <f t="shared" si="7"/>
         <v>JEFE OF. ADMINISTRATIVA</v>
       </c>
-      <c r="H28" s="214">
-        <f t="shared" ref="H28:H35" si="7">E13</f>
+      <c r="H28" s="205">
+        <f t="shared" ref="H28:H35" si="8">E13</f>
         <v>185</v>
       </c>
-      <c r="I28" s="188">
+      <c r="I28" s="180">
         <v>1</v>
       </c>
-      <c r="J28" s="184">
+      <c r="J28" s="178">
         <v>1</v>
       </c>
-      <c r="K28" s="184">
+      <c r="K28" s="178">
         <v>1</v>
       </c>
-      <c r="L28" s="184">
+      <c r="L28" s="178">
         <v>1</v>
       </c>
-      <c r="M28" s="184">
+      <c r="M28" s="178">
         <v>1</v>
       </c>
-      <c r="N28" s="220">
+      <c r="N28" s="211">
         <v>1</v>
       </c>
-      <c r="O28" s="221">
+      <c r="O28" s="212">
         <v>1</v>
       </c>
-      <c r="P28" s="196">
+      <c r="P28" s="188">
         <v>1</v>
       </c>
-      <c r="Q28" s="209">
+      <c r="Q28" s="200">
         <f t="shared" si="2"/>
         <v>1480</v>
       </c>
@@ -16992,7 +17650,7 @@
       <c r="Z28" s="159"/>
       <c r="AA28" s="159"/>
       <c r="AB28" s="159"/>
-      <c r="AC28" s="183">
+      <c r="AC28" s="296">
         <f>SUM(AC20:AC27)</f>
         <v>4662</v>
       </c>
@@ -17003,40 +17661,40 @@
       <c r="C29" s="141"/>
       <c r="D29" s="142"/>
       <c r="E29" s="142"/>
-      <c r="F29" s="219"/>
-      <c r="G29" s="191" t="str">
-        <f t="shared" si="6"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="183" t="str">
+        <f t="shared" si="7"/>
         <v>ASISTENTE OF.ADMINIS.</v>
       </c>
-      <c r="H29" s="214">
-        <f t="shared" si="7"/>
+      <c r="H29" s="205">
+        <f t="shared" si="8"/>
         <v>111</v>
       </c>
-      <c r="I29" s="188">
+      <c r="I29" s="180">
         <v>2</v>
       </c>
-      <c r="J29" s="184">
+      <c r="J29" s="178">
         <v>2</v>
       </c>
-      <c r="K29" s="184">
+      <c r="K29" s="178">
         <v>2</v>
       </c>
-      <c r="L29" s="184">
+      <c r="L29" s="178">
         <v>2</v>
       </c>
-      <c r="M29" s="184">
+      <c r="M29" s="178">
         <v>2</v>
       </c>
-      <c r="N29" s="220">
+      <c r="N29" s="211">
         <v>2</v>
       </c>
-      <c r="O29" s="221">
+      <c r="O29" s="212">
         <v>2</v>
       </c>
-      <c r="P29" s="196">
+      <c r="P29" s="188">
         <v>2</v>
       </c>
-      <c r="Q29" s="209">
+      <c r="Q29" s="200">
         <f t="shared" si="2"/>
         <v>1776</v>
       </c>
@@ -17047,40 +17705,40 @@
       <c r="C30" s="143" t="s">
         <v>861</v>
       </c>
-      <c r="F30" s="219"/>
-      <c r="G30" s="191" t="str">
-        <f t="shared" si="6"/>
+      <c r="F30" s="210"/>
+      <c r="G30" s="183" t="str">
+        <f t="shared" si="7"/>
         <v>SECRETARIA</v>
       </c>
-      <c r="H30" s="214">
-        <f t="shared" si="7"/>
+      <c r="H30" s="205">
+        <f t="shared" si="8"/>
         <v>52</v>
       </c>
-      <c r="I30" s="188">
+      <c r="I30" s="180">
         <v>1</v>
       </c>
-      <c r="J30" s="184">
+      <c r="J30" s="178">
         <v>1</v>
       </c>
-      <c r="K30" s="184">
+      <c r="K30" s="178">
         <v>1</v>
       </c>
-      <c r="L30" s="184">
+      <c r="L30" s="178">
         <v>1</v>
       </c>
-      <c r="M30" s="184">
+      <c r="M30" s="178">
         <v>1</v>
       </c>
-      <c r="N30" s="220">
+      <c r="N30" s="211">
         <v>1</v>
       </c>
-      <c r="O30" s="221">
+      <c r="O30" s="212">
         <v>1</v>
       </c>
-      <c r="P30" s="196">
+      <c r="P30" s="188">
         <v>1</v>
       </c>
-      <c r="Q30" s="209">
+      <c r="Q30" s="200">
         <f t="shared" si="2"/>
         <v>416</v>
       </c>
@@ -17090,41 +17748,41 @@
       <c r="B31" s="139"/>
       <c r="C31" s="141"/>
       <c r="D31" s="142"/>
-      <c r="E31" s="218"/>
-      <c r="F31" s="219"/>
-      <c r="G31" s="191" t="str">
-        <f t="shared" si="6"/>
+      <c r="E31" s="209"/>
+      <c r="F31" s="210"/>
+      <c r="G31" s="183" t="str">
+        <f t="shared" si="7"/>
         <v>JUNIOR</v>
       </c>
-      <c r="H31" s="214">
-        <f t="shared" si="7"/>
+      <c r="H31" s="205">
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
-      <c r="I31" s="188">
+      <c r="I31" s="180">
         <v>2</v>
       </c>
-      <c r="J31" s="184">
+      <c r="J31" s="178">
         <v>6</v>
       </c>
-      <c r="K31" s="184">
+      <c r="K31" s="178">
         <v>8</v>
       </c>
-      <c r="L31" s="184">
+      <c r="L31" s="178">
         <v>8</v>
       </c>
-      <c r="M31" s="184">
+      <c r="M31" s="178">
         <v>9</v>
       </c>
-      <c r="N31" s="220">
+      <c r="N31" s="211">
         <v>10</v>
       </c>
-      <c r="O31" s="221">
+      <c r="O31" s="212">
         <v>10</v>
       </c>
-      <c r="P31" s="196">
+      <c r="P31" s="188">
         <v>5</v>
       </c>
-      <c r="Q31" s="209">
+      <c r="Q31" s="200">
         <f t="shared" si="2"/>
         <v>1334</v>
       </c>
@@ -17135,56 +17793,56 @@
       <c r="C32" s="141"/>
       <c r="D32" s="142"/>
       <c r="E32" s="142"/>
-      <c r="F32" s="219"/>
-      <c r="G32" s="191" t="str">
-        <f t="shared" si="6"/>
+      <c r="F32" s="210"/>
+      <c r="G32" s="183" t="str">
+        <f t="shared" si="7"/>
         <v xml:space="preserve">CONDUCTOR  </v>
       </c>
-      <c r="H32" s="214">
-        <f t="shared" si="7"/>
+      <c r="H32" s="205">
+        <f t="shared" si="8"/>
         <v>59</v>
       </c>
-      <c r="I32" s="188">
+      <c r="I32" s="180">
         <v>1</v>
       </c>
-      <c r="J32" s="184">
+      <c r="J32" s="178">
         <v>1</v>
       </c>
-      <c r="K32" s="184">
+      <c r="K32" s="178">
         <v>1</v>
       </c>
-      <c r="L32" s="184">
+      <c r="L32" s="178">
         <v>1</v>
       </c>
-      <c r="M32" s="184">
+      <c r="M32" s="178">
         <v>1</v>
       </c>
-      <c r="N32" s="220">
+      <c r="N32" s="211">
         <v>2</v>
       </c>
-      <c r="O32" s="221">
+      <c r="O32" s="212">
         <v>2</v>
       </c>
-      <c r="P32" s="196">
+      <c r="P32" s="188">
         <v>1</v>
       </c>
-      <c r="Q32" s="209">
+      <c r="Q32" s="200">
         <f t="shared" si="2"/>
         <v>590</v>
       </c>
-      <c r="R32" s="245" t="s">
+      <c r="R32" s="238" t="s">
         <v>867</v>
       </c>
-      <c r="S32" s="241">
+      <c r="S32" s="217">
         <f>T32/8</f>
         <v>87145875</v>
       </c>
-      <c r="T32" s="238">
+      <c r="T32" s="235">
         <f>Q41*27000</f>
         <v>697167000</v>
       </c>
-      <c r="U32" s="238"/>
-      <c r="W32" s="244">
+      <c r="U32" s="235"/>
+      <c r="W32" s="218">
         <f>Q41</f>
         <v>25821</v>
       </c>
@@ -17195,53 +17853,53 @@
       <c r="C33" s="143"/>
       <c r="D33" s="142"/>
       <c r="E33" s="142"/>
-      <c r="F33" s="219"/>
-      <c r="G33" s="191" t="str">
-        <f t="shared" si="6"/>
+      <c r="F33" s="210"/>
+      <c r="G33" s="183" t="str">
+        <f t="shared" si="7"/>
         <v>JEFE TALLER MANTENCION</v>
       </c>
-      <c r="H33" s="214">
-        <f t="shared" si="7"/>
+      <c r="H33" s="205">
+        <f t="shared" si="8"/>
         <v>148</v>
       </c>
-      <c r="I33" s="188">
+      <c r="I33" s="180">
         <v>1</v>
       </c>
-      <c r="J33" s="184">
+      <c r="J33" s="178">
         <v>1</v>
       </c>
-      <c r="K33" s="184">
+      <c r="K33" s="178">
         <v>1</v>
       </c>
-      <c r="L33" s="184">
+      <c r="L33" s="178">
         <v>1</v>
       </c>
-      <c r="M33" s="184">
+      <c r="M33" s="178">
         <v>1</v>
       </c>
-      <c r="N33" s="220">
+      <c r="N33" s="211">
         <v>1</v>
       </c>
-      <c r="O33" s="221">
+      <c r="O33" s="212">
         <v>1</v>
       </c>
-      <c r="P33" s="196">
+      <c r="P33" s="188">
         <v>1</v>
       </c>
-      <c r="Q33" s="209">
+      <c r="Q33" s="200">
         <f t="shared" si="2"/>
         <v>1184</v>
       </c>
-      <c r="R33" s="245"/>
-      <c r="S33" s="240">
+      <c r="R33" s="238"/>
+      <c r="S33" s="216">
         <v>450000</v>
       </c>
-      <c r="T33" s="243">
+      <c r="T33" s="237">
         <f>S33*8</f>
         <v>3600000</v>
       </c>
-      <c r="U33" s="242"/>
-      <c r="W33" s="244">
+      <c r="U33" s="236"/>
+      <c r="W33" s="218">
         <f>T33/27000</f>
         <v>133.33333333333334</v>
       </c>
@@ -17251,53 +17909,53 @@
       <c r="B34" s="139"/>
       <c r="C34" s="141"/>
       <c r="E34" s="142"/>
-      <c r="F34" s="219"/>
-      <c r="G34" s="191" t="str">
-        <f t="shared" si="6"/>
+      <c r="F34" s="210"/>
+      <c r="G34" s="183" t="str">
+        <f t="shared" si="7"/>
         <v>ELECTRICO</v>
       </c>
-      <c r="H34" s="214">
-        <f t="shared" si="7"/>
+      <c r="H34" s="205">
+        <f t="shared" si="8"/>
         <v>111</v>
       </c>
-      <c r="I34" s="188">
+      <c r="I34" s="180">
         <v>1</v>
       </c>
-      <c r="J34" s="184">
+      <c r="J34" s="178">
         <v>1</v>
       </c>
-      <c r="K34" s="184">
+      <c r="K34" s="178">
         <v>1</v>
       </c>
-      <c r="L34" s="184">
+      <c r="L34" s="178">
         <v>1</v>
       </c>
-      <c r="M34" s="184">
+      <c r="M34" s="178">
         <v>1</v>
       </c>
-      <c r="N34" s="220">
+      <c r="N34" s="211">
         <v>1</v>
       </c>
-      <c r="O34" s="221">
+      <c r="O34" s="212">
         <v>1</v>
       </c>
-      <c r="P34" s="196">
+      <c r="P34" s="188">
         <v>1</v>
       </c>
-      <c r="Q34" s="209">
+      <c r="Q34" s="200">
         <f t="shared" si="2"/>
         <v>888</v>
       </c>
-      <c r="R34" s="245"/>
-      <c r="S34" s="240">
+      <c r="R34" s="238"/>
+      <c r="S34" s="216">
         <v>100000</v>
       </c>
-      <c r="T34" s="243">
+      <c r="T34" s="237">
         <f>S34*8</f>
         <v>800000</v>
       </c>
-      <c r="U34" s="242"/>
-      <c r="W34" s="244">
+      <c r="U34" s="236"/>
+      <c r="W34" s="218">
         <f>T34/27000</f>
         <v>29.62962962962963</v>
       </c>
@@ -17309,39 +17967,39 @@
       <c r="D35" s="142"/>
       <c r="E35" s="142"/>
       <c r="F35" s="121"/>
-      <c r="G35" s="192" t="str">
-        <f t="shared" si="6"/>
+      <c r="G35" s="184" t="str">
+        <f t="shared" si="7"/>
         <v>MECANICO</v>
       </c>
-      <c r="H35" s="215">
-        <f t="shared" si="7"/>
+      <c r="H35" s="206">
+        <f t="shared" si="8"/>
         <v>111</v>
       </c>
-      <c r="I35" s="189">
+      <c r="I35" s="181">
         <v>1</v>
       </c>
-      <c r="J35" s="185">
+      <c r="J35" s="179">
         <v>1</v>
       </c>
-      <c r="K35" s="185">
+      <c r="K35" s="179">
         <v>1</v>
       </c>
-      <c r="L35" s="185">
+      <c r="L35" s="179">
         <v>1</v>
       </c>
-      <c r="M35" s="185">
+      <c r="M35" s="179">
         <v>1</v>
       </c>
-      <c r="N35" s="222">
+      <c r="N35" s="213">
         <v>1</v>
       </c>
-      <c r="O35" s="223">
+      <c r="O35" s="214">
         <v>1</v>
       </c>
-      <c r="P35" s="197">
+      <c r="P35" s="189">
         <v>1</v>
       </c>
-      <c r="Q35" s="210">
+      <c r="Q35" s="201">
         <f t="shared" si="2"/>
         <v>888</v>
       </c>
@@ -17353,20 +18011,20 @@
       <c r="D36" s="142"/>
       <c r="E36" s="142"/>
       <c r="F36" s="121"/>
-      <c r="G36" s="190" t="str">
-        <f t="shared" si="6"/>
+      <c r="G36" s="182" t="str">
+        <f t="shared" si="7"/>
         <v>OTROS GASTOS</v>
       </c>
-      <c r="H36" s="216"/>
-      <c r="I36" s="195"/>
-      <c r="J36" s="195"/>
-      <c r="K36" s="195"/>
-      <c r="L36" s="195"/>
-      <c r="M36" s="195"/>
-      <c r="N36" s="195"/>
-      <c r="O36" s="195"/>
-      <c r="P36" s="195"/>
-      <c r="Q36" s="211"/>
+      <c r="H36" s="207"/>
+      <c r="I36" s="187"/>
+      <c r="J36" s="187"/>
+      <c r="K36" s="187"/>
+      <c r="L36" s="187"/>
+      <c r="M36" s="187"/>
+      <c r="N36" s="187"/>
+      <c r="O36" s="187"/>
+      <c r="P36" s="187"/>
+      <c r="Q36" s="202"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="127"/>
@@ -17375,39 +18033,39 @@
       <c r="D37" s="142"/>
       <c r="E37" s="142"/>
       <c r="F37" s="121"/>
-      <c r="G37" s="191" t="str">
-        <f t="shared" si="6"/>
+      <c r="G37" s="183" t="str">
+        <f t="shared" si="7"/>
         <v>ARRIENDO CAMIONETA (MES)</v>
       </c>
-      <c r="H37" s="214">
+      <c r="H37" s="205">
         <f>E22</f>
         <v>75</v>
       </c>
-      <c r="I37" s="188">
+      <c r="I37" s="180">
         <v>1</v>
       </c>
-      <c r="J37" s="184">
+      <c r="J37" s="178">
         <v>1</v>
       </c>
-      <c r="K37" s="184">
+      <c r="K37" s="178">
         <v>1</v>
       </c>
-      <c r="L37" s="184">
+      <c r="L37" s="178">
         <v>1</v>
       </c>
-      <c r="M37" s="184">
+      <c r="M37" s="178">
         <v>1</v>
       </c>
-      <c r="N37" s="220">
+      <c r="N37" s="211">
         <v>2</v>
       </c>
-      <c r="O37" s="221">
+      <c r="O37" s="212">
         <v>2</v>
       </c>
-      <c r="P37" s="196">
+      <c r="P37" s="188">
         <v>1</v>
       </c>
-      <c r="Q37" s="209">
+      <c r="Q37" s="200">
         <f>SUM(I37:P37)*H37</f>
         <v>750</v>
       </c>
@@ -17418,47 +18076,47 @@
       <c r="C38" s="141"/>
       <c r="D38" s="142"/>
       <c r="E38" s="142"/>
-      <c r="G38" s="191" t="str">
-        <f t="shared" si="6"/>
+      <c r="G38" s="183" t="str">
+        <f t="shared" si="7"/>
         <v>ARRIENDO GRUA</v>
       </c>
-      <c r="H38" s="214">
-        <f t="shared" ref="H38:H40" si="8">E23</f>
+      <c r="H38" s="205">
+        <f t="shared" ref="H38:H40" si="9">E23</f>
         <v>297</v>
       </c>
-      <c r="I38" s="188">
+      <c r="I38" s="180">
         <v>0</v>
       </c>
-      <c r="J38" s="184">
+      <c r="J38" s="178">
         <v>0</v>
       </c>
-      <c r="K38" s="184">
+      <c r="K38" s="178">
         <v>2</v>
       </c>
-      <c r="L38" s="184">
+      <c r="L38" s="178">
         <v>2</v>
       </c>
-      <c r="M38" s="184">
+      <c r="M38" s="178">
         <v>2</v>
       </c>
-      <c r="N38" s="184">
+      <c r="N38" s="178">
         <v>2</v>
       </c>
-      <c r="O38" s="196">
+      <c r="O38" s="188">
         <v>2</v>
       </c>
-      <c r="P38" s="196">
+      <c r="P38" s="188">
         <v>2</v>
       </c>
-      <c r="Q38" s="209">
+      <c r="Q38" s="200">
         <f>SUM(I38:P38)*H38</f>
         <v>3564</v>
       </c>
-      <c r="S38" s="236" t="s">
+      <c r="S38" s="234" t="s">
         <v>859</v>
       </c>
-      <c r="T38" s="236"/>
-      <c r="U38" s="236"/>
+      <c r="T38" s="234"/>
+      <c r="U38" s="234"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="125"/>
@@ -17466,38 +18124,38 @@
       <c r="C39" s="142"/>
       <c r="D39" s="142"/>
       <c r="E39" s="142"/>
-      <c r="G39" s="191" t="s">
+      <c r="G39" s="183" t="s">
         <v>863</v>
       </c>
-      <c r="H39" s="214">
-        <f t="shared" si="8"/>
+      <c r="H39" s="205">
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="I39" s="188">
+      <c r="I39" s="180">
         <v>1</v>
       </c>
-      <c r="J39" s="184">
+      <c r="J39" s="178">
         <v>1</v>
       </c>
-      <c r="K39" s="184">
+      <c r="K39" s="178">
         <v>1</v>
       </c>
-      <c r="L39" s="184">
+      <c r="L39" s="178">
         <v>1</v>
       </c>
-      <c r="M39" s="184">
+      <c r="M39" s="178">
         <v>1</v>
       </c>
-      <c r="N39" s="184">
+      <c r="N39" s="178">
         <v>1</v>
       </c>
-      <c r="O39" s="196">
+      <c r="O39" s="188">
         <v>1</v>
       </c>
-      <c r="P39" s="196">
+      <c r="P39" s="188">
         <v>1</v>
       </c>
-      <c r="Q39" s="209">
+      <c r="Q39" s="200">
         <f>SUM(I39:P39)*H39</f>
         <v>48</v>
       </c>
@@ -17508,38 +18166,38 @@
       <c r="C40" s="143"/>
       <c r="D40" s="142"/>
       <c r="E40" s="142"/>
-      <c r="G40" s="199" t="s">
+      <c r="G40" s="190" t="s">
         <v>864</v>
       </c>
-      <c r="H40" s="217">
-        <f t="shared" si="8"/>
+      <c r="H40" s="208">
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="I40" s="200">
+      <c r="I40" s="191">
         <v>1</v>
       </c>
-      <c r="J40" s="201">
+      <c r="J40" s="192">
         <v>1</v>
       </c>
-      <c r="K40" s="201">
+      <c r="K40" s="192">
         <v>1</v>
       </c>
-      <c r="L40" s="201">
+      <c r="L40" s="192">
         <v>1</v>
       </c>
-      <c r="M40" s="201">
+      <c r="M40" s="192">
         <v>1</v>
       </c>
-      <c r="N40" s="201">
+      <c r="N40" s="192">
         <v>1</v>
       </c>
-      <c r="O40" s="202">
+      <c r="O40" s="193">
         <v>1</v>
       </c>
-      <c r="P40" s="202">
+      <c r="P40" s="193">
         <v>1</v>
       </c>
-      <c r="Q40" s="212">
+      <c r="Q40" s="203">
         <f>SUM(I40:P40)*H40</f>
         <v>64</v>
       </c>
@@ -17550,43 +18208,43 @@
       <c r="C41" s="143"/>
       <c r="D41" s="142"/>
       <c r="E41" s="142"/>
-      <c r="G41" s="205" t="s">
+      <c r="G41" s="196" t="s">
         <v>858</v>
       </c>
-      <c r="H41" s="206"/>
-      <c r="I41" s="207">
-        <f t="shared" ref="I41:P41" si="9">SUMPRODUCT(I22:I40,$H$22:$H$40)</f>
+      <c r="H41" s="197"/>
+      <c r="I41" s="198">
+        <f t="shared" ref="I41:P41" si="10">SUMPRODUCT(I22:I40,$H$22:$H$40)</f>
         <v>2281</v>
       </c>
-      <c r="J41" s="207">
-        <f t="shared" si="9"/>
+      <c r="J41" s="198">
+        <f t="shared" si="10"/>
         <v>2558</v>
       </c>
-      <c r="K41" s="207">
-        <f t="shared" si="9"/>
+      <c r="K41" s="198">
+        <f t="shared" si="10"/>
         <v>3013</v>
       </c>
-      <c r="L41" s="207">
-        <f t="shared" si="9"/>
+      <c r="L41" s="198">
+        <f t="shared" si="10"/>
         <v>3077.75</v>
       </c>
-      <c r="M41" s="207">
-        <f t="shared" si="9"/>
+      <c r="M41" s="198">
+        <f t="shared" si="10"/>
         <v>3618.75</v>
       </c>
-      <c r="N41" s="207">
-        <f t="shared" si="9"/>
+      <c r="N41" s="198">
+        <f t="shared" si="10"/>
         <v>4293.75</v>
       </c>
-      <c r="O41" s="207">
-        <f t="shared" si="9"/>
+      <c r="O41" s="198">
+        <f t="shared" si="10"/>
         <v>3905.25</v>
       </c>
-      <c r="P41" s="207">
-        <f t="shared" si="9"/>
+      <c r="P41" s="198">
+        <f t="shared" si="10"/>
         <v>3073.5</v>
       </c>
-      <c r="Q41" s="208">
+      <c r="Q41" s="199">
         <f>SUM(Q21:Q40)</f>
         <v>25821</v>
       </c>
@@ -17607,10 +18265,10 @@
       <c r="S43" s="122" t="s">
         <v>865</v>
       </c>
-      <c r="T43" s="242" t="s">
+      <c r="T43" s="236" t="s">
         <v>866</v>
       </c>
-      <c r="U43" s="242"/>
+      <c r="U43" s="236"/>
       <c r="W43" s="122" t="s">
         <v>868</v>
       </c>
@@ -17627,12 +18285,12 @@
       <c r="R44" s="122" t="s">
         <v>861</v>
       </c>
-      <c r="S44" s="241"/>
-      <c r="T44" s="243">
+      <c r="S44" s="217"/>
+      <c r="T44" s="237">
         <v>3274824326</v>
       </c>
-      <c r="U44" s="243"/>
-      <c r="W44" s="248">
+      <c r="U44" s="237"/>
+      <c r="W44" s="221">
         <f>ROUNDUP(T44/27000,0)</f>
         <v>121290</v>
       </c>
@@ -17643,26 +18301,26 @@
       <c r="C45" s="143"/>
       <c r="D45" s="142"/>
       <c r="E45" s="142"/>
-      <c r="G45" s="224" t="s">
+      <c r="G45" s="215" t="s">
         <v>860</v>
       </c>
-      <c r="H45" s="237">
+      <c r="H45" s="230">
         <f>0.02*T44</f>
         <v>65496486.520000003</v>
       </c>
-      <c r="I45" s="237"/>
-      <c r="J45" s="237"/>
+      <c r="I45" s="230"/>
+      <c r="J45" s="230"/>
       <c r="R45" s="122" t="s">
         <v>871</v>
       </c>
-      <c r="S45" s="241"/>
-      <c r="T45" s="243">
+      <c r="S45" s="217"/>
+      <c r="T45" s="237">
         <f>T44*0.08</f>
         <v>261985946.08000001</v>
       </c>
-      <c r="U45" s="243"/>
-      <c r="W45" s="248">
-        <f t="shared" ref="W45:W52" si="10">ROUNDUP(T45/27000,0)</f>
+      <c r="U45" s="237"/>
+      <c r="W45" s="221">
+        <f t="shared" ref="W45:W52" si="11">ROUNDUP(T45/27000,0)</f>
         <v>9704</v>
       </c>
     </row>
@@ -17675,20 +18333,20 @@
       <c r="R46" s="122" t="s">
         <v>867</v>
       </c>
-      <c r="S46" s="241">
+      <c r="S46" s="217">
         <f>SUM(S32:S34)</f>
         <v>87695875</v>
       </c>
-      <c r="T46" s="243">
+      <c r="T46" s="237">
         <f>SUM(T32:U34)</f>
         <v>701567000</v>
       </c>
-      <c r="U46" s="243"/>
-      <c r="W46" s="248">
-        <f t="shared" si="10"/>
+      <c r="U46" s="237"/>
+      <c r="W46" s="221">
+        <f t="shared" si="11"/>
         <v>25984</v>
       </c>
-      <c r="X46" s="246">
+      <c r="X46" s="219">
         <f>T46/$T$44</f>
         <v>0.21423042281383126</v>
       </c>
@@ -17699,8 +18357,8 @@
       <c r="C47" s="141"/>
       <c r="D47" s="142"/>
       <c r="E47" s="142"/>
-      <c r="S47" s="240"/>
-      <c r="W47" s="248"/>
+      <c r="S47" s="216"/>
+      <c r="W47" s="221"/>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="127"/>
@@ -17711,17 +18369,17 @@
       <c r="R48" s="122" t="s">
         <v>870</v>
       </c>
-      <c r="S48" s="240"/>
-      <c r="T48" s="243">
+      <c r="S48" s="216"/>
+      <c r="T48" s="237">
         <f>0.1*SUM(T44:U46)</f>
         <v>423837727.208</v>
       </c>
-      <c r="U48" s="243"/>
-      <c r="W48" s="248">
-        <f t="shared" si="10"/>
+      <c r="U48" s="237"/>
+      <c r="W48" s="221">
+        <f t="shared" si="11"/>
         <v>15698</v>
       </c>
-      <c r="X48" s="246">
+      <c r="X48" s="219">
         <f>T48/$T$44</f>
         <v>0.12942304228138313</v>
       </c>
@@ -17735,16 +18393,16 @@
       <c r="R49" s="122" t="s">
         <v>869</v>
       </c>
-      <c r="T49" s="237">
+      <c r="T49" s="230">
         <f>0.02*SUM(T44:U46)</f>
         <v>84767545.441599995</v>
       </c>
-      <c r="U49" s="237"/>
-      <c r="W49" s="248">
-        <f t="shared" si="10"/>
+      <c r="U49" s="230"/>
+      <c r="W49" s="221">
+        <f t="shared" si="11"/>
         <v>3140</v>
       </c>
-      <c r="X49" s="246">
+      <c r="X49" s="219">
         <f>T49/$T$44</f>
         <v>2.5884608456276624E-2</v>
       </c>
@@ -17758,13 +18416,13 @@
       <c r="R50" s="122" t="s">
         <v>873</v>
       </c>
-      <c r="T50" s="237">
+      <c r="T50" s="230">
         <f>SUM(T44:U49)</f>
         <v>4746982544.7296</v>
       </c>
-      <c r="U50" s="237"/>
-      <c r="W50" s="248">
-        <f t="shared" si="10"/>
+      <c r="U50" s="230"/>
+      <c r="W50" s="221">
+        <f t="shared" si="11"/>
         <v>175815</v>
       </c>
     </row>
@@ -17787,24 +18445,24 @@
       <c r="M52" s="122">
         <v>5682</v>
       </c>
-      <c r="N52" s="238">
+      <c r="N52" s="235">
         <f>M52*2700</f>
         <v>15341400</v>
       </c>
-      <c r="O52" s="238"/>
+      <c r="O52" s="235"/>
       <c r="R52" s="122" t="s">
         <v>874</v>
       </c>
-      <c r="T52" s="237">
+      <c r="T52" s="230">
         <f>T50*0.19</f>
         <v>901926683.49862397</v>
       </c>
-      <c r="U52" s="237"/>
-      <c r="W52" s="248">
-        <f t="shared" si="10"/>
+      <c r="U52" s="230"/>
+      <c r="W52" s="221">
+        <f t="shared" si="11"/>
         <v>33405</v>
       </c>
-      <c r="X52" s="246">
+      <c r="X52" s="219">
         <f>T52/$T$44</f>
         <v>0.27541223397478326</v>
       </c>
@@ -17814,15 +18472,15 @@
       <c r="C53" s="141"/>
       <c r="D53" s="142"/>
       <c r="E53" s="142"/>
-      <c r="V53" s="247"/>
+      <c r="V53" s="220"/>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" s="125"/>
-      <c r="T54" s="237">
+      <c r="T54" s="230">
         <f>SUM(T50:U52)</f>
         <v>5648909228.2282238</v>
       </c>
-      <c r="U54" s="237"/>
+      <c r="U54" s="230"/>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" s="127"/>
@@ -17850,6 +18508,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="T54:U54"/>
     <mergeCell ref="T50:U50"/>
     <mergeCell ref="T52:U52"/>
     <mergeCell ref="B21:E21"/>
@@ -17866,7 +18525,6 @@
     <mergeCell ref="T46:U46"/>
     <mergeCell ref="T49:U49"/>
     <mergeCell ref="T45:U45"/>
-    <mergeCell ref="T54:U54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -17878,11 +18536,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177AA903-641F-4476-B876-AFE68A75CB77}">
   <dimension ref="B3:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="146"/>
@@ -18205,4 +18863,583 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3061437A-C47F-4BDF-9E4C-71A33370AA75}">
+  <dimension ref="B2:Z25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.88671875" style="240" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="240" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="240" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="11.5546875" style="240"/>
+    <col min="11" max="11" width="30.5546875" style="240" customWidth="1"/>
+    <col min="12" max="16" width="11.5546875" style="240"/>
+    <col min="17" max="17" width="25.109375" style="240" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" style="240" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.21875" style="240" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="11.5546875" style="240"/>
+    <col min="22" max="22" width="16.5546875" style="240" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.21875" style="240" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.77734375" style="240" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.5546875" style="240"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q3" s="252" t="s">
+        <v>887</v>
+      </c>
+      <c r="R3" s="252" t="s">
+        <v>891</v>
+      </c>
+      <c r="S3" s="252" t="s">
+        <v>877</v>
+      </c>
+      <c r="T3" s="252" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="4" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="252" t="s">
+        <v>876</v>
+      </c>
+      <c r="C4" s="253" t="s">
+        <v>877</v>
+      </c>
+      <c r="D4" s="254" t="s">
+        <v>878</v>
+      </c>
+      <c r="K4" s="258" t="s">
+        <v>805</v>
+      </c>
+      <c r="L4" s="277" t="s">
+        <v>806</v>
+      </c>
+      <c r="M4" s="278" t="s">
+        <v>807</v>
+      </c>
+      <c r="N4" s="279"/>
+      <c r="P4" s="300"/>
+      <c r="Q4" s="301" t="s">
+        <v>888</v>
+      </c>
+      <c r="R4" s="304">
+        <v>87145875</v>
+      </c>
+      <c r="S4" s="304">
+        <v>697167000</v>
+      </c>
+      <c r="T4" s="307">
+        <v>25821</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="243" t="s">
+        <v>875</v>
+      </c>
+      <c r="C5" s="246">
+        <f t="shared" ref="C5:C9" si="0">D5*27000</f>
+        <v>67601790</v>
+      </c>
+      <c r="D5" s="241">
+        <v>2503.77</v>
+      </c>
+      <c r="K5" s="290"/>
+      <c r="L5" s="280" t="s">
+        <v>885</v>
+      </c>
+      <c r="M5" s="281" t="s">
+        <v>885</v>
+      </c>
+      <c r="N5" s="282" t="s">
+        <v>809</v>
+      </c>
+      <c r="P5" s="300"/>
+      <c r="Q5" s="302" t="s">
+        <v>889</v>
+      </c>
+      <c r="R5" s="305">
+        <v>450000</v>
+      </c>
+      <c r="S5" s="305">
+        <v>3600000</v>
+      </c>
+      <c r="T5" s="308">
+        <v>133.33333333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="244" t="s">
+        <v>879</v>
+      </c>
+      <c r="C6" s="247">
+        <f t="shared" si="0"/>
+        <v>2005959060</v>
+      </c>
+      <c r="D6" s="242">
+        <v>74294.78</v>
+      </c>
+      <c r="K6" s="289" t="s">
+        <v>810</v>
+      </c>
+      <c r="L6" s="268">
+        <v>5000000</v>
+      </c>
+      <c r="M6" s="283">
+        <v>10000000</v>
+      </c>
+      <c r="N6" s="284">
+        <v>370</v>
+      </c>
+      <c r="P6" s="300"/>
+      <c r="Q6" s="303" t="s">
+        <v>890</v>
+      </c>
+      <c r="R6" s="306">
+        <v>100000</v>
+      </c>
+      <c r="S6" s="306">
+        <v>800000</v>
+      </c>
+      <c r="T6" s="309">
+        <v>29.62962962962963</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="244" t="s">
+        <v>880</v>
+      </c>
+      <c r="C7" s="247">
+        <f t="shared" si="0"/>
+        <v>734277420</v>
+      </c>
+      <c r="D7" s="242">
+        <v>27195.46</v>
+      </c>
+      <c r="K7" s="259" t="s">
+        <v>811</v>
+      </c>
+      <c r="L7" s="271">
+        <v>3500000</v>
+      </c>
+      <c r="M7" s="256">
+        <v>7000000</v>
+      </c>
+      <c r="N7" s="285">
+        <v>259</v>
+      </c>
+      <c r="Q7" s="310" t="s">
+        <v>892</v>
+      </c>
+      <c r="R7" s="311">
+        <f>SUM(R4:R6)</f>
+        <v>87695875</v>
+      </c>
+      <c r="S7" s="311">
+        <f t="shared" ref="S7:T7" si="1">SUM(S4:S6)</f>
+        <v>701567000</v>
+      </c>
+      <c r="T7" s="312">
+        <f t="shared" si="1"/>
+        <v>25983.962962962964</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="244" t="s">
+        <v>881</v>
+      </c>
+      <c r="C8" s="247">
+        <f t="shared" si="0"/>
+        <v>6223770</v>
+      </c>
+      <c r="D8" s="242">
+        <v>230.51</v>
+      </c>
+      <c r="K8" s="259" t="s">
+        <v>812</v>
+      </c>
+      <c r="L8" s="271">
+        <v>2500000</v>
+      </c>
+      <c r="M8" s="256">
+        <v>5000000</v>
+      </c>
+      <c r="N8" s="285">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="244" t="s">
+        <v>882</v>
+      </c>
+      <c r="C9" s="247">
+        <f t="shared" si="0"/>
+        <v>460762290</v>
+      </c>
+      <c r="D9" s="242">
+        <v>17065.27</v>
+      </c>
+      <c r="K9" s="259" t="s">
+        <v>813</v>
+      </c>
+      <c r="L9" s="271">
+        <v>2500000</v>
+      </c>
+      <c r="M9" s="256">
+        <v>5000000</v>
+      </c>
+      <c r="N9" s="285">
+        <v>185</v>
+      </c>
+      <c r="W9" s="335" t="s">
+        <v>865</v>
+      </c>
+      <c r="X9" s="336" t="s">
+        <v>877</v>
+      </c>
+      <c r="Y9" s="336" t="s">
+        <v>878</v>
+      </c>
+      <c r="Z9" s="337" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="249" t="s">
+        <v>883</v>
+      </c>
+      <c r="C10" s="250">
+        <f>D10*27000</f>
+        <v>3274824330</v>
+      </c>
+      <c r="D10" s="251">
+        <f>SUM(D5:D9)</f>
+        <v>121289.79000000001</v>
+      </c>
+      <c r="K10" s="260" t="s">
+        <v>814</v>
+      </c>
+      <c r="L10" s="271">
+        <v>2500000</v>
+      </c>
+      <c r="M10" s="256">
+        <v>5000000</v>
+      </c>
+      <c r="N10" s="285">
+        <v>185</v>
+      </c>
+      <c r="V10" s="243" t="s">
+        <v>897</v>
+      </c>
+      <c r="W10" s="313"/>
+      <c r="X10" s="314">
+        <v>3274824326</v>
+      </c>
+      <c r="Y10" s="315">
+        <v>121290</v>
+      </c>
+      <c r="Z10" s="316"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="K11" s="260" t="s">
+        <v>815</v>
+      </c>
+      <c r="L11" s="271">
+        <v>3500000</v>
+      </c>
+      <c r="M11" s="256">
+        <v>7000000</v>
+      </c>
+      <c r="N11" s="285">
+        <v>259</v>
+      </c>
+      <c r="V11" s="244" t="s">
+        <v>893</v>
+      </c>
+      <c r="W11" s="317"/>
+      <c r="X11" s="318">
+        <v>261985946.08000001</v>
+      </c>
+      <c r="Y11" s="319">
+        <v>9704</v>
+      </c>
+      <c r="Z11" s="320"/>
+    </row>
+    <row r="12" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K12" s="260" t="s">
+        <v>816</v>
+      </c>
+      <c r="L12" s="271">
+        <v>2500000</v>
+      </c>
+      <c r="M12" s="256">
+        <v>5000000</v>
+      </c>
+      <c r="N12" s="285">
+        <v>185</v>
+      </c>
+      <c r="V12" s="245" t="s">
+        <v>887</v>
+      </c>
+      <c r="W12" s="322">
+        <v>87695875</v>
+      </c>
+      <c r="X12" s="323">
+        <v>701567000</v>
+      </c>
+      <c r="Y12" s="324">
+        <v>25984</v>
+      </c>
+      <c r="Z12" s="333">
+        <v>0.21423042281383101</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="K13" s="260" t="s">
+        <v>817</v>
+      </c>
+      <c r="L13" s="271">
+        <v>1500000</v>
+      </c>
+      <c r="M13" s="256">
+        <v>3000000</v>
+      </c>
+      <c r="N13" s="285">
+        <v>111</v>
+      </c>
+      <c r="V13" s="243" t="s">
+        <v>894</v>
+      </c>
+      <c r="W13" s="313"/>
+      <c r="X13" s="314">
+        <v>423837727.208</v>
+      </c>
+      <c r="Y13" s="315">
+        <v>15698</v>
+      </c>
+      <c r="Z13" s="332">
+        <v>0.12942304228138313</v>
+      </c>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="K14" s="260" t="s">
+        <v>818</v>
+      </c>
+      <c r="L14" s="271">
+        <v>700000</v>
+      </c>
+      <c r="M14" s="256">
+        <v>1400000</v>
+      </c>
+      <c r="N14" s="285">
+        <v>52</v>
+      </c>
+      <c r="V14" s="244" t="s">
+        <v>895</v>
+      </c>
+      <c r="W14" s="317"/>
+      <c r="X14" s="318">
+        <v>84767545.441599995</v>
+      </c>
+      <c r="Y14" s="319">
+        <v>3140</v>
+      </c>
+      <c r="Z14" s="321">
+        <v>2.5884608456276624E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K15" s="260" t="s">
+        <v>819</v>
+      </c>
+      <c r="L15" s="271">
+        <v>600000</v>
+      </c>
+      <c r="M15" s="255">
+        <f>L15*2</f>
+        <v>1200000</v>
+      </c>
+      <c r="N15" s="285">
+        <f>ROUNDUP(L15/27000,0)</f>
+        <v>23</v>
+      </c>
+      <c r="V15" s="245" t="s">
+        <v>873</v>
+      </c>
+      <c r="W15" s="322"/>
+      <c r="X15" s="323">
+        <v>4746982544.7296</v>
+      </c>
+      <c r="Y15" s="324">
+        <v>175815</v>
+      </c>
+      <c r="Z15" s="333"/>
+    </row>
+    <row r="16" spans="2:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="260" t="s">
+        <v>820</v>
+      </c>
+      <c r="L16" s="271">
+        <v>800000</v>
+      </c>
+      <c r="M16" s="256">
+        <v>1600000</v>
+      </c>
+      <c r="N16" s="285">
+        <v>59</v>
+      </c>
+      <c r="V16" s="248" t="s">
+        <v>898</v>
+      </c>
+      <c r="W16" s="325"/>
+      <c r="X16" s="326">
+        <v>901926683.49862397</v>
+      </c>
+      <c r="Y16" s="327">
+        <v>33405</v>
+      </c>
+      <c r="Z16" s="334">
+        <v>0.27541223397478326</v>
+      </c>
+    </row>
+    <row r="17" spans="11:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="261" t="s">
+        <v>821</v>
+      </c>
+      <c r="L17" s="271">
+        <v>2000000</v>
+      </c>
+      <c r="M17" s="256">
+        <v>4000000</v>
+      </c>
+      <c r="N17" s="285">
+        <v>148</v>
+      </c>
+      <c r="V17" s="249" t="s">
+        <v>896</v>
+      </c>
+      <c r="W17" s="328"/>
+      <c r="X17" s="329">
+        <v>5648909228.2282238</v>
+      </c>
+      <c r="Y17" s="330">
+        <f>X17/27000</f>
+        <v>209218.86030474902</v>
+      </c>
+      <c r="Z17" s="331"/>
+    </row>
+    <row r="18" spans="11:26" x14ac:dyDescent="0.25">
+      <c r="K18" s="261" t="s">
+        <v>822</v>
+      </c>
+      <c r="L18" s="271">
+        <v>1500000</v>
+      </c>
+      <c r="M18" s="256">
+        <v>3000000</v>
+      </c>
+      <c r="N18" s="285">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="11:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K19" s="263" t="s">
+        <v>823</v>
+      </c>
+      <c r="L19" s="286">
+        <v>1500000</v>
+      </c>
+      <c r="M19" s="287">
+        <v>3000000</v>
+      </c>
+      <c r="N19" s="288">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="11:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="265" t="s">
+        <v>824</v>
+      </c>
+      <c r="L20" s="266"/>
+      <c r="M20" s="266"/>
+      <c r="N20" s="267"/>
+    </row>
+    <row r="21" spans="11:26" x14ac:dyDescent="0.25">
+      <c r="K21" s="264" t="s">
+        <v>825</v>
+      </c>
+      <c r="L21" s="268">
+        <v>2000000</v>
+      </c>
+      <c r="M21" s="269" t="s">
+        <v>884</v>
+      </c>
+      <c r="N21" s="270">
+        <f>ROUNDUP(L21/27000,0)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="11:26" x14ac:dyDescent="0.25">
+      <c r="K22" s="261" t="s">
+        <v>826</v>
+      </c>
+      <c r="L22" s="271">
+        <v>8000000</v>
+      </c>
+      <c r="M22" s="272" t="s">
+        <v>884</v>
+      </c>
+      <c r="N22" s="273">
+        <f>ROUNDUP(L22/27000,0)</f>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="23" spans="11:26" x14ac:dyDescent="0.25">
+      <c r="K23" s="261" t="s">
+        <v>886</v>
+      </c>
+      <c r="L23" s="271">
+        <v>150000</v>
+      </c>
+      <c r="M23" s="257" t="s">
+        <v>884</v>
+      </c>
+      <c r="N23" s="273">
+        <f>ROUNDUP(L23/27000,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="11:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K24" s="262" t="s">
+        <v>828</v>
+      </c>
+      <c r="L24" s="274">
+        <v>200000</v>
+      </c>
+      <c r="M24" s="275" t="s">
+        <v>884</v>
+      </c>
+      <c r="N24" s="276">
+        <f>ROUNDUP(L24/27000,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="11:26" x14ac:dyDescent="0.25">
+      <c r="M25" s="209"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="P4:P6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>